<commit_message>
Modificacion del proyecto de gimnasio 20211122_1115
</commit_message>
<xml_diff>
--- a/module/Administracion/view/administracion/mensualidad/plantilla_reporte_mensualidad.xlsx
+++ b/module/Administracion/view/administracion/mensualidad/plantilla_reporte_mensualidad.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gimnasio\module\Administracion\view\administracion\mensualidad\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2755396-E20F-44DC-9DE0-8B71CE536A16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20496" windowHeight="7692" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19420" windowHeight="7690"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -83,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-240A]\ #,##0"/>
   </numFmts>
@@ -137,7 +131,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -307,55 +301,43 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -386,26 +368,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>845820</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96EA430F-4938-4564-88B8-C968DE938F37}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -424,100 +400,16 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5303520" y="30480"/>
-          <a:ext cx="1783080" cy="1120140"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="774700" cy="774700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="190500" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="70000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5273039" cy="1142999"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectángulo 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F115429-54FD-4212-9DF9-0CA0B569C149}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15240" y="22860"/>
-          <a:ext cx="5273039" cy="1142999"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="16200000" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="obliqueBottomRight"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="es-ES" sz="5400" b="1" cap="none" spc="0">
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="bg1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="12700" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </a:rPr>
-            <a:t>POPGYM</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -776,185 +668,185 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="10" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <pane xSplit="9" ySplit="10" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="35.21875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="14" style="17" customWidth="1"/>
-    <col min="6" max="6" width="13" style="25" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" style="17" customWidth="1"/>
-    <col min="9" max="9" width="14.88671875" style="17" customWidth="1"/>
-    <col min="10" max="10" width="15.5546875" style="17" customWidth="1"/>
+    <col min="1" max="1" width="7.6328125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="14" style="15" customWidth="1"/>
+    <col min="6" max="6" width="13" style="19" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="14.90625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="15" customWidth="1"/>
     <col min="11" max="11" width="12" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.5546875" style="1"/>
+    <col min="12" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.399999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+    <row r="1" spans="1:12" ht="17.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+    <row r="2" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="3" spans="1:12" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+    <row r="3" spans="1:12" ht="11" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+    <row r="4" spans="1:12" ht="11.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
+    <row r="5" spans="1:12" ht="7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="13"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:12" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="10" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="10" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="11" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="29">
+      <c r="I7" s="25">
         <f>SUM(F11:F1048576)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.65" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="22" t="s">
         <v>3</v>
       </c>
       <c r="L9" s="2"/>
@@ -973,7 +865,7 @@
       <c r="L10" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A10:J10" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A10:J10"/>
   <mergeCells count="4">
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="I6:K6"/>

</xml_diff>